<commit_message>
ebay search test case
</commit_message>
<xml_diff>
--- a/com.bmwusa/src/test/resources/test_data.xlsx
+++ b/com.bmwusa/src/test/resources/test_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abdul\IdeaProjects\SeleniumBootcamp\com.bmwusa\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F948BF3D-F77E-4113-BA48-E2338F82FCD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{752E5EBC-A5B0-41D0-AD07-973D7D73AACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3863" yWindow="1943" windowWidth="16200" windowHeight="9307" xr2:uid="{F15093DB-1D47-4F84-BB97-98EA09F74ECD}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{F15093DB-1D47-4F84-BB97-98EA09F74ECD}"/>
   </bookViews>
   <sheets>
     <sheet name="login_bmw" sheetId="1" r:id="rId1"/>
@@ -419,12 +419,13 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A4" sqref="A4:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">

</xml_diff>